<commit_message>
update and extend the ICA results table: networks and SVM performance
</commit_message>
<xml_diff>
--- a/ICA_selection_table.xlsx
+++ b/ICA_selection_table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kajin\Documents\_\3\Thesis\ESO\eso\ICA\results\20240124\ICASSO_fovselect5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kajin\PhD\ESO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D9DBE5-CD36-41BE-801C-9FA20F474AA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF6CB95-E7CF-4B4D-A8EB-A5CB0C813247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="15370" activeTab="1" xr2:uid="{322E97A4-5E11-4D2E-B660-A47433EC49A8}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{322E97A4-5E11-4D2E-B660-A47433EC49A8}"/>
   </bookViews>
   <sheets>
     <sheet name="ikem" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="28">
   <si>
     <t>r</t>
   </si>
@@ -55,15 +55,81 @@
   <si>
     <t xml:space="preserve">C no. </t>
   </si>
+  <si>
+    <t>SVM accuracy using only this C</t>
+  </si>
+  <si>
+    <t>artifact</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>anterior DMN</t>
+  </si>
+  <si>
+    <t>anterior and posterior DMN</t>
+  </si>
+  <si>
+    <t>primary audiory cortex</t>
+  </si>
+  <si>
+    <t>precuneal + cuneal + V2</t>
+  </si>
+  <si>
+    <t>visual cortex</t>
+  </si>
+  <si>
+    <t>middle frontal gyrus (CEN)</t>
+  </si>
+  <si>
+    <t>inferior parietal lobule, somatosenzory</t>
+  </si>
+  <si>
+    <t>part of precuneus</t>
+  </si>
+  <si>
+    <t>part of superior frontal gyrus</t>
+  </si>
+  <si>
+    <t>included in classification, t-test not significant</t>
+  </si>
+  <si>
+    <t>included in classification + significant t-test</t>
+  </si>
+  <si>
+    <t>high performance (70+)</t>
+  </si>
+  <si>
+    <t>cuneal cortex</t>
+  </si>
+  <si>
+    <t>network / area</t>
+  </si>
+  <si>
+    <t>somatosenzory and motor cortex</t>
+  </si>
+  <si>
+    <t>precuneal cortex, ACC</t>
+  </si>
+  <si>
+    <t>medial prefrontal cortex, ACC</t>
+  </si>
+  <si>
+    <t>sec. somatosenzory cortex</t>
+  </si>
+  <si>
+    <t>superior parietal lobule</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0000"/>
-  </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,6 +141,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -107,12 +179,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -245,11 +317,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -287,9 +383,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -302,7 +395,58 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -639,10 +783,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B24398A-0CC5-4EF1-9295-0298D3C81F93}">
-  <dimension ref="A2:E37"/>
+  <dimension ref="A2:M37"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -650,9 +794,11 @@
     <col min="1" max="1" width="19.453125" style="1" customWidth="1"/>
     <col min="2" max="4" width="6.6328125" style="2" customWidth="1"/>
     <col min="5" max="5" width="6.6328125" customWidth="1"/>
+    <col min="6" max="6" width="35.6328125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="28.26953125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="9" t="s">
         <v>3</v>
       </c>
@@ -665,26 +811,32 @@
       <c r="E2" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="2:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="F2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B3" s="4">
         <v>1</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="13">
         <v>0.96689999999999998</v>
       </c>
       <c r="D3" s="10">
         <v>-0.49180000000000001</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="16">
         <v>-4.83</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B4" s="6">
         <v>2</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="14">
         <v>0.97150000000000003</v>
       </c>
       <c r="D4" s="11">
@@ -693,12 +845,16 @@
       <c r="E4" s="11">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="L4" s="28"/>
+      <c r="M4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B5" s="6">
         <v>3</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="14">
         <v>0.97799999999999998</v>
       </c>
       <c r="D5" s="11">
@@ -708,25 +864,29 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B6" s="6">
         <v>4</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="14">
         <v>0.97170000000000001</v>
       </c>
       <c r="D6" s="11">
         <v>-0.1368</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="18">
         <v>1.49</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="L6" s="29"/>
+      <c r="M6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B7" s="5">
         <v>5</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="14">
         <v>0.97040000000000004</v>
       </c>
       <c r="D7" s="12">
@@ -735,26 +895,36 @@
       <c r="E7" s="11">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F7" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="19">
+        <v>51.27</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B8" s="6">
         <v>6</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="14">
         <v>0.97650000000000003</v>
       </c>
       <c r="D8" s="11">
         <v>-0.17100000000000001</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="20">
         <v>-0.72</v>
       </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="L8" s="30"/>
+      <c r="M8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B9" s="7">
         <v>7</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="14">
         <v>0.97070000000000001</v>
       </c>
       <c r="D9" s="12">
@@ -763,40 +933,46 @@
       <c r="E9" s="12">
         <v>-6.23</v>
       </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F9" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="25">
+        <v>71.33</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B10" s="6">
         <v>8</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="14">
         <v>0.97529999999999994</v>
       </c>
       <c r="D10" s="11">
         <v>0.14829999999999999</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="10">
         <v>0.86</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B11" s="6">
         <v>9</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="14">
         <v>0.97330000000000005</v>
       </c>
       <c r="D11" s="11">
         <v>-0.2268</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="22">
         <v>-6.23</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B12" s="7">
         <v>10</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="14">
         <v>0.97270000000000001</v>
       </c>
       <c r="D12" s="12">
@@ -805,26 +981,32 @@
       <c r="E12" s="12">
         <v>3.91</v>
       </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F12" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B13" s="6">
         <v>11</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="14">
         <v>0.97330000000000005</v>
       </c>
       <c r="D13" s="11">
         <v>0.19769999999999999</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="16">
         <v>6.99</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B14" s="6">
         <v>12</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="14">
         <v>0.97389999999999999</v>
       </c>
       <c r="D14" s="11">
@@ -834,11 +1016,11 @@
         <v>2.2799999999999998</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B15" s="6">
         <v>13</v>
       </c>
-      <c r="C15" s="15">
+      <c r="C15" s="14">
         <v>0.97489999999999999</v>
       </c>
       <c r="D15" s="11">
@@ -848,25 +1030,25 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B16" s="6">
         <v>14</v>
       </c>
-      <c r="C16" s="15">
+      <c r="C16" s="14">
         <v>0.96799999999999997</v>
       </c>
       <c r="D16" s="11">
         <v>0.1467</v>
       </c>
-      <c r="E16" s="12">
+      <c r="E16" s="22">
         <v>-2.1</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B17" s="7">
         <v>15</v>
       </c>
-      <c r="C17" s="15">
+      <c r="C17" s="14">
         <v>0.97119999999999995</v>
       </c>
       <c r="D17" s="12">
@@ -875,12 +1057,18 @@
       <c r="E17" s="12">
         <v>-7.42</v>
       </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F17" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" s="27">
+        <v>70.319999999999993</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B18" s="5">
         <v>16</v>
       </c>
-      <c r="C18" s="15">
+      <c r="C18" s="14">
         <v>0.96689999999999998</v>
       </c>
       <c r="D18" s="12">
@@ -889,40 +1077,49 @@
       <c r="E18" s="11">
         <v>-0.46</v>
       </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F18" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="19">
+        <v>16.45</v>
+      </c>
+      <c r="H18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B19" s="6">
         <v>17</v>
       </c>
-      <c r="C19" s="15">
+      <c r="C19" s="14">
         <v>0.97740000000000005</v>
       </c>
       <c r="D19" s="11">
         <v>0.39369999999999999</v>
       </c>
-      <c r="E19" s="12">
+      <c r="E19" s="16">
         <v>1.89</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B20" s="6">
         <v>18</v>
       </c>
-      <c r="C20" s="15">
+      <c r="C20" s="14">
         <v>0.97130000000000005</v>
       </c>
       <c r="D20" s="11">
         <v>0.33629999999999999</v>
       </c>
-      <c r="E20" s="11">
+      <c r="E20" s="18">
         <v>0.33</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B21" s="7">
         <v>19</v>
       </c>
-      <c r="C21" s="15">
+      <c r="C21" s="14">
         <v>0.96350000000000002</v>
       </c>
       <c r="D21" s="12">
@@ -931,12 +1128,18 @@
       <c r="E21" s="12">
         <v>-5.48</v>
       </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F21" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="21">
+        <v>67.44</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B22" s="7">
         <v>20</v>
       </c>
-      <c r="C22" s="15">
+      <c r="C22" s="14">
         <v>0.96930000000000005</v>
       </c>
       <c r="D22" s="12">
@@ -945,26 +1148,32 @@
       <c r="E22" s="12">
         <v>2.4</v>
       </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F22" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="21">
+        <v>66.38</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B23" s="6">
         <v>21</v>
       </c>
-      <c r="C23" s="15">
+      <c r="C23" s="14">
         <v>0.96550000000000002</v>
       </c>
       <c r="D23" s="11">
         <v>-0.24679999999999999</v>
       </c>
-      <c r="E23" s="12">
+      <c r="E23" s="23">
         <v>3.56</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B24" s="7">
         <v>22</v>
       </c>
-      <c r="C24" s="15">
+      <c r="C24" s="14">
         <v>0.97409999999999997</v>
       </c>
       <c r="D24" s="12">
@@ -973,26 +1182,32 @@
       <c r="E24" s="12">
         <v>7.13</v>
       </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F24" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="25">
+        <v>74.52</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B25" s="6">
         <v>23</v>
       </c>
-      <c r="C25" s="15">
+      <c r="C25" s="14">
         <v>0.95379999999999998</v>
       </c>
       <c r="D25" s="11">
         <v>-0.1678</v>
       </c>
-      <c r="E25" s="11">
+      <c r="E25" s="20">
         <v>1.29</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B26" s="7">
         <v>24</v>
       </c>
-      <c r="C26" s="15">
+      <c r="C26" s="14">
         <v>0.96579999999999999</v>
       </c>
       <c r="D26" s="12">
@@ -1001,26 +1216,32 @@
       <c r="E26" s="12">
         <v>3.32</v>
       </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F26" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" s="21">
+        <v>56.89</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B27" s="6">
         <v>25</v>
       </c>
-      <c r="C27" s="15">
+      <c r="C27" s="14">
         <v>0.96440000000000003</v>
       </c>
       <c r="D27" s="11">
         <v>0.25169999999999998</v>
       </c>
-      <c r="E27" s="12">
+      <c r="E27" s="16">
         <v>3.8</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B28" s="6">
         <v>26</v>
       </c>
-      <c r="C28" s="15">
+      <c r="C28" s="14">
         <v>0.97360000000000002</v>
       </c>
       <c r="D28" s="11">
@@ -1030,11 +1251,11 @@
         <v>-1.65</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B29" s="6">
         <v>27</v>
       </c>
-      <c r="C29" s="15">
+      <c r="C29" s="14">
         <v>0.9617</v>
       </c>
       <c r="D29" s="11">
@@ -1044,11 +1265,11 @@
         <v>-6.85</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B30" s="6">
         <v>28</v>
       </c>
-      <c r="C30" s="15">
+      <c r="C30" s="14">
         <v>0.93799999999999994</v>
       </c>
       <c r="D30" s="11">
@@ -1058,25 +1279,25 @@
         <v>1.42</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B31" s="6">
         <v>29</v>
       </c>
-      <c r="C31" s="15">
+      <c r="C31" s="14">
         <v>0.94789999999999996</v>
       </c>
       <c r="D31" s="11">
         <v>0.42820000000000003</v>
       </c>
-      <c r="E31" s="11">
+      <c r="E31" s="18">
         <v>1.67</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B32" s="7">
         <v>30</v>
       </c>
-      <c r="C32" s="15">
+      <c r="C32" s="14">
         <v>0.95020000000000004</v>
       </c>
       <c r="D32" s="12">
@@ -1085,12 +1306,18 @@
       <c r="E32" s="12">
         <v>-2.6</v>
       </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F32" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G32" s="21">
+        <v>64.06</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B33" s="7">
         <v>31</v>
       </c>
-      <c r="C33" s="15">
+      <c r="C33" s="14">
         <v>0.93459999999999999</v>
       </c>
       <c r="D33" s="12">
@@ -1099,26 +1326,32 @@
       <c r="E33" s="12">
         <v>3.43</v>
       </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F33" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="G33" s="21">
+        <v>63.46</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B34" s="6">
         <v>32</v>
       </c>
-      <c r="C34" s="15">
+      <c r="C34" s="14">
         <v>0.9446</v>
       </c>
       <c r="D34" s="11">
         <v>0.36930000000000002</v>
       </c>
-      <c r="E34" s="12">
+      <c r="E34" s="16">
         <v>2.97</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B35" s="6">
         <v>33</v>
       </c>
-      <c r="C35" s="15">
+      <c r="C35" s="14">
         <v>0.92079999999999995</v>
       </c>
       <c r="D35" s="11">
@@ -1128,11 +1361,11 @@
         <v>5.16</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B36" s="6">
         <v>34</v>
       </c>
-      <c r="C36" s="15">
+      <c r="C36" s="14">
         <v>0.92969999999999997</v>
       </c>
       <c r="D36" s="11">
@@ -1142,11 +1375,11 @@
         <v>2.96</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B37" s="6">
         <v>35</v>
       </c>
-      <c r="C37" s="16">
+      <c r="C37" s="15">
         <v>0.83169999999999999</v>
       </c>
       <c r="D37" s="11">
@@ -1163,10 +1396,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576DB81D-AF32-4CCF-96BD-3CD21ABF5628}">
-  <dimension ref="A2:G37"/>
+  <dimension ref="A2:M37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1174,9 +1407,11 @@
     <col min="1" max="1" width="19.453125" style="1" customWidth="1"/>
     <col min="2" max="4" width="6.6328125" style="2" customWidth="1"/>
     <col min="5" max="5" width="6.6328125" customWidth="1"/>
+    <col min="6" max="6" width="35.6328125" style="32" customWidth="1"/>
+    <col min="7" max="7" width="28.26953125" style="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
@@ -1189,12 +1424,18 @@
       <c r="E2" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="F2" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B3" s="4">
         <v>1</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="13">
         <v>0.98109999999999997</v>
       </c>
       <c r="D3" s="10">
@@ -1203,13 +1444,12 @@
       <c r="E3" s="10">
         <v>-1.37</v>
       </c>
-      <c r="G3" s="13"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B4" s="5">
         <v>2</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="14">
         <v>0.97240000000000004</v>
       </c>
       <c r="D4" s="12">
@@ -1218,13 +1458,22 @@
       <c r="E4" s="11">
         <v>-0.86</v>
       </c>
-      <c r="G4" s="13"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="F4" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="33">
+        <v>53.9</v>
+      </c>
+      <c r="L4" s="28"/>
+      <c r="M4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B5" s="5">
         <v>3</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="14">
         <v>0.97489999999999999</v>
       </c>
       <c r="D5" s="12">
@@ -1233,13 +1482,21 @@
       <c r="E5" s="11">
         <v>-0.05</v>
       </c>
-      <c r="G5" s="13"/>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="F5" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="33">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B6" s="6">
         <v>4</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="14">
         <v>0.97450000000000003</v>
       </c>
       <c r="D6" s="11">
@@ -1248,13 +1505,16 @@
       <c r="E6" s="11">
         <v>-0.98</v>
       </c>
-      <c r="G6" s="13"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="L6" s="29"/>
+      <c r="M6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B7" s="7">
         <v>5</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="14">
         <v>0.97140000000000004</v>
       </c>
       <c r="D7" s="12">
@@ -1263,13 +1523,18 @@
       <c r="E7" s="12">
         <v>-4.87</v>
       </c>
-      <c r="G7" s="13"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="F7" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B8" s="6">
         <v>6</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="14">
         <v>0.96319999999999995</v>
       </c>
       <c r="D8" s="11">
@@ -1278,13 +1543,18 @@
       <c r="E8" s="11">
         <v>0.19</v>
       </c>
-      <c r="G8" s="13"/>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="L8" s="30"/>
+      <c r="M8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B9" s="6">
         <v>7</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="14">
         <v>0.97489999999999999</v>
       </c>
       <c r="D9" s="11">
@@ -1293,13 +1563,14 @@
       <c r="E9" s="11">
         <v>-0.38</v>
       </c>
-      <c r="G9" s="13"/>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="F9" s="34"/>
+      <c r="G9" s="17"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B10" s="6">
         <v>8</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="14">
         <v>0.97019999999999995</v>
       </c>
       <c r="D10" s="11">
@@ -1308,13 +1579,14 @@
       <c r="E10" s="11">
         <v>-0.12</v>
       </c>
-      <c r="G10" s="13"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B11" s="6">
         <v>9</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="14">
         <v>0.96440000000000003</v>
       </c>
       <c r="D11" s="11">
@@ -1323,13 +1595,14 @@
       <c r="E11" s="12">
         <v>2.2999999999999998</v>
       </c>
-      <c r="G11" s="13"/>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B12" s="6">
         <v>10</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="14">
         <v>0.98240000000000005</v>
       </c>
       <c r="D12" s="11">
@@ -1338,13 +1611,14 @@
       <c r="E12" s="12">
         <v>2.37</v>
       </c>
-      <c r="G12" s="13"/>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B13" s="6">
         <v>11</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="14">
         <v>0.9657</v>
       </c>
       <c r="D13" s="11">
@@ -1353,42 +1627,50 @@
       <c r="E13" s="11">
         <v>-1.1100000000000001</v>
       </c>
-      <c r="G13" s="13"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B14" s="18">
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B14" s="7">
         <v>12</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="14">
         <v>0.96909999999999996</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="12">
+        <v>-0.72909999999999997</v>
+      </c>
+      <c r="E14" s="12">
+        <v>-4.1100000000000003</v>
+      </c>
+      <c r="F14" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="33">
+        <v>58.93</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B15" s="6">
+        <v>13</v>
+      </c>
+      <c r="C15" s="14">
+        <v>0.9627</v>
+      </c>
+      <c r="D15" s="11">
         <v>-0.1086</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E15" s="12">
         <v>-2.2599999999999998</v>
       </c>
-      <c r="G14" s="13"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B15" s="7">
-        <v>13</v>
-      </c>
-      <c r="C15" s="15">
-        <v>0.97</v>
-      </c>
-      <c r="D15" s="12">
-        <v>-0.72909999999999997</v>
-      </c>
-      <c r="E15" s="12">
-        <v>-4.1100000000000003</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B16" s="6">
         <v>14</v>
       </c>
-      <c r="C16" s="15">
+      <c r="C16" s="14">
         <v>0.9698</v>
       </c>
       <c r="D16" s="11">
@@ -1397,13 +1679,14 @@
       <c r="E16" s="12">
         <v>3.91</v>
       </c>
-      <c r="G16" s="13"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B17" s="6">
         <v>15</v>
       </c>
-      <c r="C17" s="15">
+      <c r="C17" s="14">
         <v>0.96279999999999999</v>
       </c>
       <c r="D17" s="11">
@@ -1412,13 +1695,14 @@
       <c r="E17" s="11">
         <v>1.53</v>
       </c>
-      <c r="G17" s="13"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="36"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B18" s="6">
         <v>16</v>
       </c>
-      <c r="C18" s="15">
+      <c r="C18" s="14">
         <v>0.9577</v>
       </c>
       <c r="D18" s="11">
@@ -1427,13 +1711,14 @@
       <c r="E18" s="11">
         <v>1.1399999999999999</v>
       </c>
-      <c r="G18" s="13"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B19" s="6">
         <v>17</v>
       </c>
-      <c r="C19" s="15">
+      <c r="C19" s="14">
         <v>0.97099999999999997</v>
       </c>
       <c r="D19" s="11">
@@ -1442,13 +1727,14 @@
       <c r="E19" s="11">
         <v>0.36</v>
       </c>
-      <c r="G19" s="13"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B20" s="7">
         <v>18</v>
       </c>
-      <c r="C20" s="15">
+      <c r="C20" s="14">
         <v>0.95499999999999996</v>
       </c>
       <c r="D20" s="12">
@@ -1457,13 +1743,18 @@
       <c r="E20" s="12">
         <v>-3.53</v>
       </c>
-      <c r="G20" s="13"/>
+      <c r="F20" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20" s="33">
+        <v>58.81</v>
+      </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B21" s="6">
         <v>19</v>
       </c>
-      <c r="C21" s="15">
+      <c r="C21" s="14">
         <v>0.9597</v>
       </c>
       <c r="D21" s="11">
@@ -1472,13 +1763,14 @@
       <c r="E21" s="12">
         <v>-2.02</v>
       </c>
-      <c r="G21" s="13"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="17"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B22" s="7">
         <v>20</v>
       </c>
-      <c r="C22" s="15">
+      <c r="C22" s="14">
         <v>0.93310000000000004</v>
       </c>
       <c r="D22" s="12">
@@ -1487,13 +1779,18 @@
       <c r="E22" s="12">
         <v>5.76</v>
       </c>
-      <c r="G22" s="13"/>
+      <c r="F22" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22" s="21" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B23" s="6">
         <v>21</v>
       </c>
-      <c r="C23" s="15">
+      <c r="C23" s="14">
         <v>0.9224</v>
       </c>
       <c r="D23" s="11">
@@ -1502,13 +1799,14 @@
       <c r="E23" s="12">
         <v>-2.64</v>
       </c>
-      <c r="G23" s="13"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="34"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B24" s="7">
         <v>22</v>
       </c>
-      <c r="C24" s="15">
+      <c r="C24" s="14">
         <v>0.94</v>
       </c>
       <c r="D24" s="12">
@@ -1517,13 +1815,18 @@
       <c r="E24" s="12">
         <v>2.95</v>
       </c>
-      <c r="G24" s="13"/>
+      <c r="F24" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="G24" s="21">
+        <v>55.65</v>
+      </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B25" s="7">
         <v>23</v>
       </c>
-      <c r="C25" s="15">
+      <c r="C25" s="14">
         <v>0.93149999999999999</v>
       </c>
       <c r="D25" s="12">
@@ -1532,13 +1835,18 @@
       <c r="E25" s="12">
         <v>3.53</v>
       </c>
-      <c r="G25" s="13"/>
+      <c r="F25" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="G25" s="33">
+        <v>62.04</v>
+      </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B26" s="6">
         <v>24</v>
       </c>
-      <c r="C26" s="16">
+      <c r="C26" s="15">
         <v>0.89300000000000002</v>
       </c>
       <c r="D26" s="11">
@@ -1547,13 +1855,14 @@
       <c r="E26" s="11">
         <v>1.1200000000000001</v>
       </c>
-      <c r="G26" s="13"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="17"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B27" s="6">
         <v>25</v>
       </c>
-      <c r="C27" s="16">
+      <c r="C27" s="15">
         <v>0.84799999999999998</v>
       </c>
       <c r="D27" s="12">
@@ -1562,13 +1871,14 @@
       <c r="E27" s="12">
         <v>-3.74</v>
       </c>
-      <c r="G27" s="13"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B28" s="6">
         <v>26</v>
       </c>
-      <c r="C28" s="16">
+      <c r="C28" s="15">
         <v>0.83279999999999998</v>
       </c>
       <c r="D28" s="12">
@@ -1577,13 +1887,14 @@
       <c r="E28" s="12">
         <v>4.34</v>
       </c>
-      <c r="G28" s="13"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="34"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B29" s="6">
         <v>27</v>
       </c>
-      <c r="C29" s="16">
+      <c r="C29" s="15">
         <v>0.80520000000000003</v>
       </c>
       <c r="D29" s="12">
@@ -1592,13 +1903,14 @@
       <c r="E29" s="11">
         <v>1.35</v>
       </c>
-      <c r="G29" s="13"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="34"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B30" s="6">
         <v>28</v>
       </c>
-      <c r="C30" s="16">
+      <c r="C30" s="15">
         <v>0.80569999999999997</v>
       </c>
       <c r="D30" s="12">
@@ -1607,13 +1919,14 @@
       <c r="E30" s="12">
         <v>-3.41</v>
       </c>
-      <c r="G30" s="13"/>
+      <c r="F30" s="34"/>
+      <c r="G30" s="34"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B31" s="6">
         <v>29</v>
       </c>
-      <c r="C31" s="16">
+      <c r="C31" s="15">
         <v>0.86570000000000003</v>
       </c>
       <c r="D31" s="11">
@@ -1622,13 +1935,14 @@
       <c r="E31" s="11">
         <v>1.3</v>
       </c>
-      <c r="G31" s="13"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="34"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B32" s="7">
         <v>30</v>
       </c>
-      <c r="C32" s="15">
+      <c r="C32" s="14">
         <v>0.91320000000000001</v>
       </c>
       <c r="D32" s="12">
@@ -1637,13 +1951,18 @@
       <c r="E32" s="12">
         <v>3.08</v>
       </c>
-      <c r="G32" s="13"/>
+      <c r="F32" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="G32" s="21">
+        <v>62.71</v>
+      </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B33" s="6">
         <v>31</v>
       </c>
-      <c r="C33" s="16">
+      <c r="C33" s="15">
         <v>0.78090000000000004</v>
       </c>
       <c r="D33" s="12">
@@ -1652,13 +1971,14 @@
       <c r="E33" s="12">
         <v>5.51</v>
       </c>
-      <c r="G33" s="13"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="17"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B34" s="6">
         <v>32</v>
       </c>
-      <c r="C34" s="16">
+      <c r="C34" s="15">
         <v>0.88349999999999995</v>
       </c>
       <c r="D34" s="11">
@@ -1667,13 +1987,12 @@
       <c r="E34" s="11">
         <v>-1.0900000000000001</v>
       </c>
-      <c r="G34" s="13"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B35" s="6">
         <v>33</v>
       </c>
-      <c r="C35" s="16">
+      <c r="C35" s="15">
         <v>0.83530000000000004</v>
       </c>
       <c r="D35" s="12">
@@ -1682,13 +2001,12 @@
       <c r="E35" s="12">
         <v>4.01</v>
       </c>
-      <c r="G35" s="13"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B36" s="6">
         <v>34</v>
       </c>
-      <c r="C36" s="16">
+      <c r="C36" s="15">
         <v>0.73519999999999996</v>
       </c>
       <c r="D36" s="11">
@@ -1697,13 +2015,12 @@
       <c r="E36" s="12">
         <v>2.2200000000000002</v>
       </c>
-      <c r="G36" s="13"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B37" s="6">
         <v>35</v>
       </c>
-      <c r="C37" s="16">
+      <c r="C37" s="15">
         <v>0.57750000000000001</v>
       </c>
       <c r="D37" s="11">
@@ -1712,7 +2029,6 @@
       <c r="E37" s="11">
         <v>-0.28000000000000003</v>
       </c>
-      <c r="G37" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1724,7 +2040,7 @@
   <dimension ref="A2:E37"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E37"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1752,13 +2068,13 @@
       <c r="B3" s="4">
         <v>1</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="13">
         <v>0.96230000000000004</v>
       </c>
       <c r="D3" s="10">
         <v>0.49590000000000001</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="16">
         <v>7.12</v>
       </c>
     </row>
@@ -1766,7 +2082,7 @@
       <c r="B4" s="6">
         <v>2</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="14">
         <v>0.9738</v>
       </c>
       <c r="D4" s="11">
@@ -1780,7 +2096,7 @@
       <c r="B5" s="6">
         <v>3</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="14">
         <v>0.97599999999999998</v>
       </c>
       <c r="D5" s="11">
@@ -1794,7 +2110,7 @@
       <c r="B6" s="6">
         <v>4</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="14">
         <v>0.97170000000000001</v>
       </c>
       <c r="D6" s="11">
@@ -1808,7 +2124,7 @@
       <c r="B7" s="7">
         <v>5</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="14">
         <v>0.96599999999999997</v>
       </c>
       <c r="D7" s="12">
@@ -1822,7 +2138,7 @@
       <c r="B8" s="7">
         <v>6</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="14">
         <v>0.96840000000000004</v>
       </c>
       <c r="D8" s="12">
@@ -1836,7 +2152,7 @@
       <c r="B9" s="6">
         <v>7</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="14">
         <v>0.97099999999999997</v>
       </c>
       <c r="D9" s="11">
@@ -1850,7 +2166,7 @@
       <c r="B10" s="7">
         <v>8</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="14">
         <v>0.96909999999999996</v>
       </c>
       <c r="D10" s="12">
@@ -1864,7 +2180,7 @@
       <c r="B11" s="6">
         <v>9</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="14">
         <v>0.97370000000000001</v>
       </c>
       <c r="D11" s="11">
@@ -1878,7 +2194,7 @@
       <c r="B12" s="6">
         <v>10</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="14">
         <v>0.95450000000000002</v>
       </c>
       <c r="D12" s="11">
@@ -1892,7 +2208,7 @@
       <c r="B13" s="6">
         <v>11</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="14">
         <v>0.96509999999999996</v>
       </c>
       <c r="D13" s="11">
@@ -1906,7 +2222,7 @@
       <c r="B14" s="6">
         <v>12</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="14">
         <v>0.96719999999999995</v>
       </c>
       <c r="D14" s="11">
@@ -1920,7 +2236,7 @@
       <c r="B15" s="6">
         <v>13</v>
       </c>
-      <c r="C15" s="15">
+      <c r="C15" s="14">
         <v>0.96589999999999998</v>
       </c>
       <c r="D15" s="11">
@@ -1934,7 +2250,7 @@
       <c r="B16" s="6">
         <v>14</v>
       </c>
-      <c r="C16" s="15">
+      <c r="C16" s="14">
         <v>0.95820000000000005</v>
       </c>
       <c r="D16" s="11">
@@ -1948,7 +2264,7 @@
       <c r="B17" s="6">
         <v>15</v>
       </c>
-      <c r="C17" s="15">
+      <c r="C17" s="14">
         <v>0.95930000000000004</v>
       </c>
       <c r="D17" s="11">
@@ -1962,7 +2278,7 @@
       <c r="B18" s="7">
         <v>16</v>
       </c>
-      <c r="C18" s="15">
+      <c r="C18" s="14">
         <v>0.95379999999999998</v>
       </c>
       <c r="D18" s="12">
@@ -1976,7 +2292,7 @@
       <c r="B19" s="7">
         <v>17</v>
       </c>
-      <c r="C19" s="15">
+      <c r="C19" s="14">
         <v>0.9667</v>
       </c>
       <c r="D19" s="12">
@@ -1990,7 +2306,7 @@
       <c r="B20" s="7">
         <v>18</v>
       </c>
-      <c r="C20" s="15">
+      <c r="C20" s="14">
         <v>0.93500000000000005</v>
       </c>
       <c r="D20" s="12">
@@ -2004,7 +2320,7 @@
       <c r="B21" s="6">
         <v>19</v>
       </c>
-      <c r="C21" s="15">
+      <c r="C21" s="14">
         <v>0.96699999999999997</v>
       </c>
       <c r="D21" s="11">
@@ -2018,7 +2334,7 @@
       <c r="B22" s="7">
         <v>20</v>
       </c>
-      <c r="C22" s="15">
+      <c r="C22" s="14">
         <v>0.97350000000000003</v>
       </c>
       <c r="D22" s="12">
@@ -2032,7 +2348,7 @@
       <c r="B23" s="7">
         <v>21</v>
       </c>
-      <c r="C23" s="15">
+      <c r="C23" s="14">
         <v>0.97270000000000001</v>
       </c>
       <c r="D23" s="12">
@@ -2046,7 +2362,7 @@
       <c r="B24" s="7">
         <v>22</v>
       </c>
-      <c r="C24" s="15">
+      <c r="C24" s="14">
         <v>0.9617</v>
       </c>
       <c r="D24" s="12">
@@ -2060,7 +2376,7 @@
       <c r="B25" s="6">
         <v>23</v>
       </c>
-      <c r="C25" s="15">
+      <c r="C25" s="14">
         <v>0.95499999999999996</v>
       </c>
       <c r="D25" s="11">
@@ -2074,7 +2390,7 @@
       <c r="B26" s="6">
         <v>24</v>
       </c>
-      <c r="C26" s="15">
+      <c r="C26" s="14">
         <v>0.96719999999999995</v>
       </c>
       <c r="D26" s="11">
@@ -2088,7 +2404,7 @@
       <c r="B27" s="6">
         <v>25</v>
       </c>
-      <c r="C27" s="15">
+      <c r="C27" s="14">
         <v>0.95109999999999995</v>
       </c>
       <c r="D27" s="11">
@@ -2102,7 +2418,7 @@
       <c r="B28" s="7">
         <v>26</v>
       </c>
-      <c r="C28" s="15">
+      <c r="C28" s="14">
         <v>0.95840000000000003</v>
       </c>
       <c r="D28" s="12">
@@ -2116,7 +2432,7 @@
       <c r="B29" s="6">
         <v>27</v>
       </c>
-      <c r="C29" s="15">
+      <c r="C29" s="14">
         <v>0.96360000000000001</v>
       </c>
       <c r="D29" s="11">
@@ -2130,7 +2446,7 @@
       <c r="B30" s="6">
         <v>28</v>
       </c>
-      <c r="C30" s="15">
+      <c r="C30" s="14">
         <v>0.95389999999999997</v>
       </c>
       <c r="D30" s="11">
@@ -2144,7 +2460,7 @@
       <c r="B31" s="6">
         <v>29</v>
       </c>
-      <c r="C31" s="15">
+      <c r="C31" s="14">
         <v>0.95989999999999998</v>
       </c>
       <c r="D31" s="11">
@@ -2158,7 +2474,7 @@
       <c r="B32" s="5">
         <v>30</v>
       </c>
-      <c r="C32" s="15">
+      <c r="C32" s="14">
         <v>0.92920000000000003</v>
       </c>
       <c r="D32" s="12">
@@ -2172,7 +2488,7 @@
       <c r="B33" s="5">
         <v>31</v>
       </c>
-      <c r="C33" s="15">
+      <c r="C33" s="14">
         <v>0.92249999999999999</v>
       </c>
       <c r="D33" s="12">
@@ -2186,7 +2502,7 @@
       <c r="B34" s="6">
         <v>32</v>
       </c>
-      <c r="C34" s="15">
+      <c r="C34" s="14">
         <v>0.94630000000000003</v>
       </c>
       <c r="D34" s="11">
@@ -2200,7 +2516,7 @@
       <c r="B35" s="6">
         <v>33</v>
       </c>
-      <c r="C35" s="16">
+      <c r="C35" s="15">
         <v>0.80120000000000002</v>
       </c>
       <c r="D35" s="12">
@@ -2214,7 +2530,7 @@
       <c r="B36" s="7">
         <v>34</v>
       </c>
-      <c r="C36" s="15">
+      <c r="C36" s="14">
         <v>0.9244</v>
       </c>
       <c r="D36" s="12">
@@ -2228,7 +2544,7 @@
       <c r="B37" s="6">
         <v>35</v>
       </c>
-      <c r="C37" s="16">
+      <c r="C37" s="15">
         <v>0.63819999999999999</v>
       </c>
       <c r="D37" s="12">
@@ -2248,7 +2564,7 @@
   <dimension ref="B2:O37"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="S27" sqref="S27"/>
+      <selection activeCell="G14" sqref="G14:J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2301,19 +2617,19 @@
       <c r="B3" s="4">
         <v>1</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="13">
         <v>0.96689999999999998</v>
       </c>
       <c r="D3" s="10">
         <v>-0.49180000000000001</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="16">
         <v>-4.83</v>
       </c>
       <c r="G3" s="4">
         <v>1</v>
       </c>
-      <c r="H3" s="14">
+      <c r="H3" s="13">
         <v>0.98109999999999997</v>
       </c>
       <c r="I3" s="10">
@@ -2325,13 +2641,13 @@
       <c r="L3" s="4">
         <v>1</v>
       </c>
-      <c r="M3" s="14">
+      <c r="M3" s="13">
         <v>0.96230000000000004</v>
       </c>
       <c r="N3" s="10">
         <v>0.49590000000000001</v>
       </c>
-      <c r="O3" s="17">
+      <c r="O3" s="16">
         <v>7.12</v>
       </c>
     </row>
@@ -2339,7 +2655,7 @@
       <c r="B4" s="6">
         <v>2</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="14">
         <v>0.97150000000000003</v>
       </c>
       <c r="D4" s="11">
@@ -2351,7 +2667,7 @@
       <c r="G4" s="5">
         <v>2</v>
       </c>
-      <c r="H4" s="15">
+      <c r="H4" s="14">
         <v>0.97240000000000004</v>
       </c>
       <c r="I4" s="12">
@@ -2363,7 +2679,7 @@
       <c r="L4" s="6">
         <v>2</v>
       </c>
-      <c r="M4" s="15">
+      <c r="M4" s="14">
         <v>0.9738</v>
       </c>
       <c r="N4" s="11">
@@ -2377,7 +2693,7 @@
       <c r="B5" s="6">
         <v>3</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="14">
         <v>0.97799999999999998</v>
       </c>
       <c r="D5" s="11">
@@ -2389,7 +2705,7 @@
       <c r="G5" s="5">
         <v>3</v>
       </c>
-      <c r="H5" s="15">
+      <c r="H5" s="14">
         <v>0.97489999999999999</v>
       </c>
       <c r="I5" s="12">
@@ -2401,7 +2717,7 @@
       <c r="L5" s="6">
         <v>3</v>
       </c>
-      <c r="M5" s="15">
+      <c r="M5" s="14">
         <v>0.97599999999999998</v>
       </c>
       <c r="N5" s="11">
@@ -2415,7 +2731,7 @@
       <c r="B6" s="6">
         <v>4</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="14">
         <v>0.97170000000000001</v>
       </c>
       <c r="D6" s="11">
@@ -2427,7 +2743,7 @@
       <c r="G6" s="6">
         <v>4</v>
       </c>
-      <c r="H6" s="15">
+      <c r="H6" s="14">
         <v>0.97450000000000003</v>
       </c>
       <c r="I6" s="11">
@@ -2439,7 +2755,7 @@
       <c r="L6" s="6">
         <v>4</v>
       </c>
-      <c r="M6" s="15">
+      <c r="M6" s="14">
         <v>0.97170000000000001</v>
       </c>
       <c r="N6" s="11">
@@ -2453,7 +2769,7 @@
       <c r="B7" s="5">
         <v>5</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="14">
         <v>0.97040000000000004</v>
       </c>
       <c r="D7" s="12">
@@ -2465,7 +2781,7 @@
       <c r="G7" s="7">
         <v>5</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7" s="14">
         <v>0.97140000000000004</v>
       </c>
       <c r="I7" s="12">
@@ -2477,7 +2793,7 @@
       <c r="L7" s="7">
         <v>5</v>
       </c>
-      <c r="M7" s="15">
+      <c r="M7" s="14">
         <v>0.96599999999999997</v>
       </c>
       <c r="N7" s="12">
@@ -2491,7 +2807,7 @@
       <c r="B8" s="6">
         <v>6</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="14">
         <v>0.97650000000000003</v>
       </c>
       <c r="D8" s="11">
@@ -2503,7 +2819,7 @@
       <c r="G8" s="6">
         <v>6</v>
       </c>
-      <c r="H8" s="15">
+      <c r="H8" s="14">
         <v>0.96319999999999995</v>
       </c>
       <c r="I8" s="11">
@@ -2515,7 +2831,7 @@
       <c r="L8" s="7">
         <v>6</v>
       </c>
-      <c r="M8" s="15">
+      <c r="M8" s="14">
         <v>0.96840000000000004</v>
       </c>
       <c r="N8" s="12">
@@ -2529,7 +2845,7 @@
       <c r="B9" s="7">
         <v>7</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="14">
         <v>0.97070000000000001</v>
       </c>
       <c r="D9" s="12">
@@ -2541,7 +2857,7 @@
       <c r="G9" s="6">
         <v>7</v>
       </c>
-      <c r="H9" s="15">
+      <c r="H9" s="14">
         <v>0.97489999999999999</v>
       </c>
       <c r="I9" s="11">
@@ -2553,7 +2869,7 @@
       <c r="L9" s="6">
         <v>7</v>
       </c>
-      <c r="M9" s="15">
+      <c r="M9" s="14">
         <v>0.97099999999999997</v>
       </c>
       <c r="N9" s="11">
@@ -2567,7 +2883,7 @@
       <c r="B10" s="6">
         <v>8</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="14">
         <v>0.97529999999999994</v>
       </c>
       <c r="D10" s="11">
@@ -2579,7 +2895,7 @@
       <c r="G10" s="6">
         <v>8</v>
       </c>
-      <c r="H10" s="15">
+      <c r="H10" s="14">
         <v>0.97019999999999995</v>
       </c>
       <c r="I10" s="11">
@@ -2591,7 +2907,7 @@
       <c r="L10" s="7">
         <v>8</v>
       </c>
-      <c r="M10" s="15">
+      <c r="M10" s="14">
         <v>0.96909999999999996</v>
       </c>
       <c r="N10" s="12">
@@ -2605,7 +2921,7 @@
       <c r="B11" s="6">
         <v>9</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="14">
         <v>0.97330000000000005</v>
       </c>
       <c r="D11" s="11">
@@ -2617,7 +2933,7 @@
       <c r="G11" s="6">
         <v>9</v>
       </c>
-      <c r="H11" s="15">
+      <c r="H11" s="14">
         <v>0.96440000000000003</v>
       </c>
       <c r="I11" s="11">
@@ -2629,7 +2945,7 @@
       <c r="L11" s="6">
         <v>9</v>
       </c>
-      <c r="M11" s="15">
+      <c r="M11" s="14">
         <v>0.97370000000000001</v>
       </c>
       <c r="N11" s="11">
@@ -2643,7 +2959,7 @@
       <c r="B12" s="7">
         <v>10</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="14">
         <v>0.97270000000000001</v>
       </c>
       <c r="D12" s="12">
@@ -2655,7 +2971,7 @@
       <c r="G12" s="6">
         <v>10</v>
       </c>
-      <c r="H12" s="15">
+      <c r="H12" s="14">
         <v>0.98240000000000005</v>
       </c>
       <c r="I12" s="11">
@@ -2667,7 +2983,7 @@
       <c r="L12" s="6">
         <v>10</v>
       </c>
-      <c r="M12" s="15">
+      <c r="M12" s="14">
         <v>0.95450000000000002</v>
       </c>
       <c r="N12" s="11">
@@ -2681,7 +2997,7 @@
       <c r="B13" s="6">
         <v>11</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="14">
         <v>0.97330000000000005</v>
       </c>
       <c r="D13" s="11">
@@ -2693,7 +3009,7 @@
       <c r="G13" s="6">
         <v>11</v>
       </c>
-      <c r="H13" s="15">
+      <c r="H13" s="14">
         <v>0.9657</v>
       </c>
       <c r="I13" s="11">
@@ -2705,7 +3021,7 @@
       <c r="L13" s="6">
         <v>11</v>
       </c>
-      <c r="M13" s="15">
+      <c r="M13" s="14">
         <v>0.96509999999999996</v>
       </c>
       <c r="N13" s="11">
@@ -2719,7 +3035,7 @@
       <c r="B14" s="6">
         <v>12</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="14">
         <v>0.97389999999999999</v>
       </c>
       <c r="D14" s="11">
@@ -2731,7 +3047,7 @@
       <c r="G14" s="7">
         <v>12</v>
       </c>
-      <c r="H14" s="15">
+      <c r="H14" s="14">
         <v>0.96909999999999996</v>
       </c>
       <c r="I14" s="12">
@@ -2743,7 +3059,7 @@
       <c r="L14" s="6">
         <v>12</v>
       </c>
-      <c r="M14" s="15">
+      <c r="M14" s="14">
         <v>0.96719999999999995</v>
       </c>
       <c r="N14" s="11">
@@ -2757,7 +3073,7 @@
       <c r="B15" s="6">
         <v>13</v>
       </c>
-      <c r="C15" s="15">
+      <c r="C15" s="14">
         <v>0.97489999999999999</v>
       </c>
       <c r="D15" s="11">
@@ -2769,7 +3085,7 @@
       <c r="G15" s="6">
         <v>13</v>
       </c>
-      <c r="H15" s="15">
+      <c r="H15" s="14">
         <v>0.9627</v>
       </c>
       <c r="I15" s="11">
@@ -2781,7 +3097,7 @@
       <c r="L15" s="6">
         <v>13</v>
       </c>
-      <c r="M15" s="15">
+      <c r="M15" s="14">
         <v>0.96589999999999998</v>
       </c>
       <c r="N15" s="11">
@@ -2795,7 +3111,7 @@
       <c r="B16" s="6">
         <v>14</v>
       </c>
-      <c r="C16" s="15">
+      <c r="C16" s="14">
         <v>0.96799999999999997</v>
       </c>
       <c r="D16" s="11">
@@ -2807,7 +3123,7 @@
       <c r="G16" s="6">
         <v>14</v>
       </c>
-      <c r="H16" s="15">
+      <c r="H16" s="14">
         <v>0.9698</v>
       </c>
       <c r="I16" s="11">
@@ -2819,7 +3135,7 @@
       <c r="L16" s="6">
         <v>14</v>
       </c>
-      <c r="M16" s="15">
+      <c r="M16" s="14">
         <v>0.95820000000000005</v>
       </c>
       <c r="N16" s="11">
@@ -2833,7 +3149,7 @@
       <c r="B17" s="7">
         <v>15</v>
       </c>
-      <c r="C17" s="15">
+      <c r="C17" s="14">
         <v>0.97119999999999995</v>
       </c>
       <c r="D17" s="12">
@@ -2845,7 +3161,7 @@
       <c r="G17" s="6">
         <v>15</v>
       </c>
-      <c r="H17" s="15">
+      <c r="H17" s="14">
         <v>0.96279999999999999</v>
       </c>
       <c r="I17" s="11">
@@ -2857,7 +3173,7 @@
       <c r="L17" s="6">
         <v>15</v>
       </c>
-      <c r="M17" s="15">
+      <c r="M17" s="14">
         <v>0.95930000000000004</v>
       </c>
       <c r="N17" s="11">
@@ -2871,7 +3187,7 @@
       <c r="B18" s="5">
         <v>16</v>
       </c>
-      <c r="C18" s="15">
+      <c r="C18" s="14">
         <v>0.96689999999999998</v>
       </c>
       <c r="D18" s="12">
@@ -2883,7 +3199,7 @@
       <c r="G18" s="6">
         <v>16</v>
       </c>
-      <c r="H18" s="15">
+      <c r="H18" s="14">
         <v>0.9577</v>
       </c>
       <c r="I18" s="11">
@@ -2895,7 +3211,7 @@
       <c r="L18" s="7">
         <v>16</v>
       </c>
-      <c r="M18" s="15">
+      <c r="M18" s="14">
         <v>0.95379999999999998</v>
       </c>
       <c r="N18" s="12">
@@ -2909,7 +3225,7 @@
       <c r="B19" s="6">
         <v>17</v>
       </c>
-      <c r="C19" s="15">
+      <c r="C19" s="14">
         <v>0.97740000000000005</v>
       </c>
       <c r="D19" s="11">
@@ -2921,7 +3237,7 @@
       <c r="G19" s="6">
         <v>17</v>
       </c>
-      <c r="H19" s="15">
+      <c r="H19" s="14">
         <v>0.97099999999999997</v>
       </c>
       <c r="I19" s="11">
@@ -2933,7 +3249,7 @@
       <c r="L19" s="7">
         <v>17</v>
       </c>
-      <c r="M19" s="15">
+      <c r="M19" s="14">
         <v>0.9667</v>
       </c>
       <c r="N19" s="12">
@@ -2947,7 +3263,7 @@
       <c r="B20" s="6">
         <v>18</v>
       </c>
-      <c r="C20" s="15">
+      <c r="C20" s="14">
         <v>0.97130000000000005</v>
       </c>
       <c r="D20" s="11">
@@ -2959,7 +3275,7 @@
       <c r="G20" s="7">
         <v>18</v>
       </c>
-      <c r="H20" s="15">
+      <c r="H20" s="14">
         <v>0.95499999999999996</v>
       </c>
       <c r="I20" s="12">
@@ -2971,7 +3287,7 @@
       <c r="L20" s="7">
         <v>18</v>
       </c>
-      <c r="M20" s="15">
+      <c r="M20" s="14">
         <v>0.93500000000000005</v>
       </c>
       <c r="N20" s="12">
@@ -2985,7 +3301,7 @@
       <c r="B21" s="7">
         <v>19</v>
       </c>
-      <c r="C21" s="15">
+      <c r="C21" s="14">
         <v>0.96350000000000002</v>
       </c>
       <c r="D21" s="12">
@@ -2997,7 +3313,7 @@
       <c r="G21" s="6">
         <v>19</v>
       </c>
-      <c r="H21" s="15">
+      <c r="H21" s="14">
         <v>0.9597</v>
       </c>
       <c r="I21" s="11">
@@ -3009,7 +3325,7 @@
       <c r="L21" s="6">
         <v>19</v>
       </c>
-      <c r="M21" s="15">
+      <c r="M21" s="14">
         <v>0.96699999999999997</v>
       </c>
       <c r="N21" s="11">
@@ -3023,7 +3339,7 @@
       <c r="B22" s="7">
         <v>20</v>
       </c>
-      <c r="C22" s="15">
+      <c r="C22" s="14">
         <v>0.96930000000000005</v>
       </c>
       <c r="D22" s="12">
@@ -3035,7 +3351,7 @@
       <c r="G22" s="7">
         <v>20</v>
       </c>
-      <c r="H22" s="15">
+      <c r="H22" s="14">
         <v>0.93310000000000004</v>
       </c>
       <c r="I22" s="12">
@@ -3047,7 +3363,7 @@
       <c r="L22" s="7">
         <v>20</v>
       </c>
-      <c r="M22" s="15">
+      <c r="M22" s="14">
         <v>0.97350000000000003</v>
       </c>
       <c r="N22" s="12">
@@ -3061,7 +3377,7 @@
       <c r="B23" s="6">
         <v>21</v>
       </c>
-      <c r="C23" s="15">
+      <c r="C23" s="14">
         <v>0.96550000000000002</v>
       </c>
       <c r="D23" s="11">
@@ -3073,7 +3389,7 @@
       <c r="G23" s="6">
         <v>21</v>
       </c>
-      <c r="H23" s="15">
+      <c r="H23" s="14">
         <v>0.9224</v>
       </c>
       <c r="I23" s="11">
@@ -3085,7 +3401,7 @@
       <c r="L23" s="7">
         <v>21</v>
       </c>
-      <c r="M23" s="15">
+      <c r="M23" s="14">
         <v>0.97270000000000001</v>
       </c>
       <c r="N23" s="12">
@@ -3099,7 +3415,7 @@
       <c r="B24" s="7">
         <v>22</v>
       </c>
-      <c r="C24" s="15">
+      <c r="C24" s="14">
         <v>0.97409999999999997</v>
       </c>
       <c r="D24" s="12">
@@ -3111,7 +3427,7 @@
       <c r="G24" s="7">
         <v>22</v>
       </c>
-      <c r="H24" s="15">
+      <c r="H24" s="14">
         <v>0.94</v>
       </c>
       <c r="I24" s="12">
@@ -3123,7 +3439,7 @@
       <c r="L24" s="7">
         <v>22</v>
       </c>
-      <c r="M24" s="15">
+      <c r="M24" s="14">
         <v>0.9617</v>
       </c>
       <c r="N24" s="12">
@@ -3137,7 +3453,7 @@
       <c r="B25" s="6">
         <v>23</v>
       </c>
-      <c r="C25" s="15">
+      <c r="C25" s="14">
         <v>0.95379999999999998</v>
       </c>
       <c r="D25" s="11">
@@ -3149,7 +3465,7 @@
       <c r="G25" s="7">
         <v>23</v>
       </c>
-      <c r="H25" s="15">
+      <c r="H25" s="14">
         <v>0.93149999999999999</v>
       </c>
       <c r="I25" s="12">
@@ -3161,7 +3477,7 @@
       <c r="L25" s="6">
         <v>23</v>
       </c>
-      <c r="M25" s="15">
+      <c r="M25" s="14">
         <v>0.95499999999999996</v>
       </c>
       <c r="N25" s="11">
@@ -3175,7 +3491,7 @@
       <c r="B26" s="7">
         <v>24</v>
       </c>
-      <c r="C26" s="15">
+      <c r="C26" s="14">
         <v>0.96579999999999999</v>
       </c>
       <c r="D26" s="12">
@@ -3187,7 +3503,7 @@
       <c r="G26" s="6">
         <v>24</v>
       </c>
-      <c r="H26" s="16">
+      <c r="H26" s="15">
         <v>0.89300000000000002</v>
       </c>
       <c r="I26" s="11">
@@ -3199,7 +3515,7 @@
       <c r="L26" s="6">
         <v>24</v>
       </c>
-      <c r="M26" s="15">
+      <c r="M26" s="14">
         <v>0.96719999999999995</v>
       </c>
       <c r="N26" s="11">
@@ -3213,7 +3529,7 @@
       <c r="B27" s="6">
         <v>25</v>
       </c>
-      <c r="C27" s="15">
+      <c r="C27" s="14">
         <v>0.96440000000000003</v>
       </c>
       <c r="D27" s="11">
@@ -3225,7 +3541,7 @@
       <c r="G27" s="6">
         <v>25</v>
       </c>
-      <c r="H27" s="16">
+      <c r="H27" s="15">
         <v>0.84799999999999998</v>
       </c>
       <c r="I27" s="12">
@@ -3237,7 +3553,7 @@
       <c r="L27" s="6">
         <v>25</v>
       </c>
-      <c r="M27" s="15">
+      <c r="M27" s="14">
         <v>0.95109999999999995</v>
       </c>
       <c r="N27" s="11">
@@ -3251,7 +3567,7 @@
       <c r="B28" s="6">
         <v>26</v>
       </c>
-      <c r="C28" s="15">
+      <c r="C28" s="14">
         <v>0.97360000000000002</v>
       </c>
       <c r="D28" s="11">
@@ -3263,7 +3579,7 @@
       <c r="G28" s="6">
         <v>26</v>
       </c>
-      <c r="H28" s="16">
+      <c r="H28" s="15">
         <v>0.83279999999999998</v>
       </c>
       <c r="I28" s="12">
@@ -3275,7 +3591,7 @@
       <c r="L28" s="7">
         <v>26</v>
       </c>
-      <c r="M28" s="15">
+      <c r="M28" s="14">
         <v>0.95840000000000003</v>
       </c>
       <c r="N28" s="12">
@@ -3289,7 +3605,7 @@
       <c r="B29" s="6">
         <v>27</v>
       </c>
-      <c r="C29" s="15">
+      <c r="C29" s="14">
         <v>0.9617</v>
       </c>
       <c r="D29" s="11">
@@ -3301,7 +3617,7 @@
       <c r="G29" s="6">
         <v>27</v>
       </c>
-      <c r="H29" s="16">
+      <c r="H29" s="15">
         <v>0.80520000000000003</v>
       </c>
       <c r="I29" s="12">
@@ -3313,7 +3629,7 @@
       <c r="L29" s="6">
         <v>27</v>
       </c>
-      <c r="M29" s="15">
+      <c r="M29" s="14">
         <v>0.96360000000000001</v>
       </c>
       <c r="N29" s="11">
@@ -3327,7 +3643,7 @@
       <c r="B30" s="6">
         <v>28</v>
       </c>
-      <c r="C30" s="15">
+      <c r="C30" s="14">
         <v>0.93799999999999994</v>
       </c>
       <c r="D30" s="11">
@@ -3339,7 +3655,7 @@
       <c r="G30" s="6">
         <v>28</v>
       </c>
-      <c r="H30" s="16">
+      <c r="H30" s="15">
         <v>0.80569999999999997</v>
       </c>
       <c r="I30" s="12">
@@ -3351,7 +3667,7 @@
       <c r="L30" s="6">
         <v>28</v>
       </c>
-      <c r="M30" s="15">
+      <c r="M30" s="14">
         <v>0.95389999999999997</v>
       </c>
       <c r="N30" s="11">
@@ -3365,7 +3681,7 @@
       <c r="B31" s="6">
         <v>29</v>
       </c>
-      <c r="C31" s="15">
+      <c r="C31" s="14">
         <v>0.94789999999999996</v>
       </c>
       <c r="D31" s="11">
@@ -3377,7 +3693,7 @@
       <c r="G31" s="6">
         <v>29</v>
       </c>
-      <c r="H31" s="16">
+      <c r="H31" s="15">
         <v>0.86570000000000003</v>
       </c>
       <c r="I31" s="11">
@@ -3389,7 +3705,7 @@
       <c r="L31" s="6">
         <v>29</v>
       </c>
-      <c r="M31" s="15">
+      <c r="M31" s="14">
         <v>0.95989999999999998</v>
       </c>
       <c r="N31" s="11">
@@ -3403,7 +3719,7 @@
       <c r="B32" s="7">
         <v>30</v>
       </c>
-      <c r="C32" s="15">
+      <c r="C32" s="14">
         <v>0.95020000000000004</v>
       </c>
       <c r="D32" s="12">
@@ -3415,7 +3731,7 @@
       <c r="G32" s="7">
         <v>30</v>
       </c>
-      <c r="H32" s="15">
+      <c r="H32" s="14">
         <v>0.91320000000000001</v>
       </c>
       <c r="I32" s="12">
@@ -3427,7 +3743,7 @@
       <c r="L32" s="5">
         <v>30</v>
       </c>
-      <c r="M32" s="15">
+      <c r="M32" s="14">
         <v>0.92920000000000003</v>
       </c>
       <c r="N32" s="12">
@@ -3441,7 +3757,7 @@
       <c r="B33" s="7">
         <v>31</v>
       </c>
-      <c r="C33" s="15">
+      <c r="C33" s="14">
         <v>0.93459999999999999</v>
       </c>
       <c r="D33" s="12">
@@ -3453,7 +3769,7 @@
       <c r="G33" s="6">
         <v>31</v>
       </c>
-      <c r="H33" s="16">
+      <c r="H33" s="15">
         <v>0.78090000000000004</v>
       </c>
       <c r="I33" s="12">
@@ -3465,7 +3781,7 @@
       <c r="L33" s="5">
         <v>31</v>
       </c>
-      <c r="M33" s="15">
+      <c r="M33" s="14">
         <v>0.92249999999999999</v>
       </c>
       <c r="N33" s="12">
@@ -3479,7 +3795,7 @@
       <c r="B34" s="6">
         <v>32</v>
       </c>
-      <c r="C34" s="15">
+      <c r="C34" s="14">
         <v>0.9446</v>
       </c>
       <c r="D34" s="11">
@@ -3491,7 +3807,7 @@
       <c r="G34" s="6">
         <v>32</v>
       </c>
-      <c r="H34" s="16">
+      <c r="H34" s="15">
         <v>0.88349999999999995</v>
       </c>
       <c r="I34" s="11">
@@ -3503,7 +3819,7 @@
       <c r="L34" s="6">
         <v>32</v>
       </c>
-      <c r="M34" s="15">
+      <c r="M34" s="14">
         <v>0.94630000000000003</v>
       </c>
       <c r="N34" s="11">
@@ -3517,7 +3833,7 @@
       <c r="B35" s="6">
         <v>33</v>
       </c>
-      <c r="C35" s="15">
+      <c r="C35" s="14">
         <v>0.92079999999999995</v>
       </c>
       <c r="D35" s="11">
@@ -3529,7 +3845,7 @@
       <c r="G35" s="6">
         <v>33</v>
       </c>
-      <c r="H35" s="16">
+      <c r="H35" s="15">
         <v>0.79949999999999999</v>
       </c>
       <c r="I35" s="12">
@@ -3541,7 +3857,7 @@
       <c r="L35" s="6">
         <v>33</v>
       </c>
-      <c r="M35" s="16">
+      <c r="M35" s="15">
         <v>0.80120000000000002</v>
       </c>
       <c r="N35" s="12">
@@ -3555,7 +3871,7 @@
       <c r="B36" s="6">
         <v>34</v>
       </c>
-      <c r="C36" s="15">
+      <c r="C36" s="14">
         <v>0.92969999999999997</v>
       </c>
       <c r="D36" s="11">
@@ -3567,7 +3883,7 @@
       <c r="G36" s="6">
         <v>34</v>
       </c>
-      <c r="H36" s="16">
+      <c r="H36" s="15">
         <v>0.75729999999999997</v>
       </c>
       <c r="I36" s="11">
@@ -3579,7 +3895,7 @@
       <c r="L36" s="7">
         <v>34</v>
       </c>
-      <c r="M36" s="15">
+      <c r="M36" s="14">
         <v>0.9244</v>
       </c>
       <c r="N36" s="12">
@@ -3593,7 +3909,7 @@
       <c r="B37" s="6">
         <v>35</v>
       </c>
-      <c r="C37" s="16">
+      <c r="C37" s="15">
         <v>0.83169999999999999</v>
       </c>
       <c r="D37" s="11">
@@ -3605,7 +3921,7 @@
       <c r="G37" s="6">
         <v>35</v>
       </c>
-      <c r="H37" s="16">
+      <c r="H37" s="15">
         <v>0.57750000000000001</v>
       </c>
       <c r="I37" s="11">
@@ -3617,7 +3933,7 @@
       <c r="L37" s="6">
         <v>35</v>
       </c>
-      <c r="M37" s="16">
+      <c r="M37" s="15">
         <v>0.63819999999999999</v>
       </c>
       <c r="N37" s="12">

</xml_diff>